<commit_message>
completed extraction thruogh export
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\datooda\OneDrive - EY\1-Projects\Document Understanding Training\DUDiplomaExercise-UiPath\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{9ADA8DC4-5857-4028-85F6-AD0B97B8590E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{95B2E47D-C094-479A-8758-93B79554A33C}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{9ADA8DC4-5857-4028-85F6-AD0B97B8590E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{D45D64EE-A968-49B4-B250-2370B90EBD09}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -135,13 +135,13 @@
     <t>ApiKey</t>
   </si>
   <si>
-    <t>DocumentUnderstandingApiKey</t>
-  </si>
-  <si>
-    <t>Name of the API key credential stored in the Windows Credential Manager or Orchestrator.</t>
-  </si>
-  <si>
     <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name.</t>
+  </si>
+  <si>
+    <t>API Key for Document Understanding</t>
+  </si>
+  <si>
+    <t>WrkgP7yV4ratarJL3XRlKgGr0xbijIdiYbHXSsiIJkJ82U4DeTF3dOrKIjngT7aVjAsJXDIVmPCUSBnveWghHw==</t>
   </si>
 </sst>
 </file>
@@ -513,7 +513,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -577,7 +579,7 @@
         <v>29</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
@@ -606,7 +608,7 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
Add my API key
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\datooda\OneDrive - EY\1-Projects\Document Understanding Training\DUDiplomaExercise-UiPath\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\datooda\Downloads\DUDiplomaExercise-UiPath\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{9ADA8DC4-5857-4028-85F6-AD0B97B8590E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{D45D64EE-A968-49B4-B250-2370B90EBD09}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8146B4EA-F512-4FA0-82BB-031A9ED383D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3420" yWindow="0" windowWidth="23115" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -141,7 +141,7 @@
     <t>API Key for Document Understanding</t>
   </si>
   <si>
-    <t>WrkgP7yV4ratarJL3XRlKgGr0xbijIdiYbHXSsiIJkJ82U4DeTF3dOrKIjngT7aVjAsJXDIVmPCUSBnveWghHw==</t>
+    <t>7GQ8RyXzrL1Ifqx+Jkc257nap1ndAZekltwJqJ/gyxtqc+hrutCqkT1l3JRtEiqQ</t>
   </si>
 </sst>
 </file>
@@ -514,7 +514,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>